<commit_message>
final working copy for demo
</commit_message>
<xml_diff>
--- a/app/assets/data/Chapters.xlsx
+++ b/app/assets/data/Chapters.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26009"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SrinjoyMajumdar/Documents/AtsaCorp/ImagineDragons/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Chapters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Introduction to astronomy. Goes over basics of things we see everyday in the sky and general observations.</t>
   </si>
@@ -90,13 +85,22 @@
   </si>
   <si>
     <t>How molecules and even cells make up our bodies.</t>
+  </si>
+  <si>
+    <t>Astronomy Stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goes over all stars </t>
+  </si>
+  <si>
+    <t>World History Wars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -107,6 +111,22 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,8 +149,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -143,7 +175,19 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -199,7 +243,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,7 +278,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -411,7 +455,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,13 +463,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
@@ -433,7 +477,7 @@
     <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="32">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -450,7 +494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="32">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -467,7 +511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="16">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -484,7 +528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -501,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15">
       <c r="A5" s="1">
         <v>5</v>
       </c>
@@ -518,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15">
       <c r="A6" s="1">
         <v>6</v>
       </c>
@@ -535,7 +579,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="30">
       <c r="A7" s="1">
         <v>7</v>
       </c>
@@ -552,7 +596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="1">
         <v>8</v>
       </c>
@@ -569,7 +613,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="30">
       <c r="A9" s="1">
         <v>9</v>
       </c>
@@ -586,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="30">
       <c r="A10" s="1">
         <v>10</v>
       </c>
@@ -603,7 +647,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -620,7 +664,47 @@
         <v>2</v>
       </c>
     </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="1">
+        <v>13</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>